<commit_message>
Fix data point in 2019 toy budget data
</commit_message>
<xml_diff>
--- a/data/city_budgets_2019.xlsx
+++ b/data/city_budgets_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tumgoren/code/stanford/stanford-progj-2020/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{999D6B0C-D587-1F47-8D3B-766A787371A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45D0E30-C2F3-D245-B0AA-5B44D4F01694}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4220" yWindow="1520" windowWidth="26440" windowHeight="15440" xr2:uid="{0EC23F8D-8D95-1A44-95C3-DCF9FD0C060E}"/>
   </bookViews>
@@ -414,7 +414,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224FDE9F-3065-9142-AA5F-B3138DBDC7E1}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -496,7 +498,7 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>95000000</v>
+        <v>9500000</v>
       </c>
       <c r="D6">
         <v>2019</v>

</xml_diff>